<commit_message>
Merged PR 9627: BP-813 : Affiliate Mapping for True Independent Stations
CR Task : https://jira.crossmw.com/browse/BP-1255
</commit_message>
<xml_diff>
--- a/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ImportStationMappings/CadentBroadcastStationList_DifferentOwnership.xlsx
+++ b/Source/Tam/MaestroTests/SupportTests/Services.Broadcast.IntegrationTests/Files/ImportStationMappings/CadentBroadcastStationList_DifferentOwnership.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\sroibu\Source\Repos\Broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ImportStationMappings\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\broadcast\Source\Tam\MaestroTests\SupportTests\Services.Broadcast.IntegrationTests\Files\ImportStationMappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C46C5710-A393-4980-A284-0602D20BBBDF}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8538C0-6C56-464E-9F25-30ECA0AC3925}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4A9EC11D-1DEC-477A-A2B3-C5EC15B2E530}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27375" windowHeight="16440" xr2:uid="{4A9EC11D-1DEC-477A-A2B3-C5EC15B2E530}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>SigmaCallLetters</t>
   </si>
   <si>
-    <t>Affiliation Mismatch Note</t>
-  </si>
-  <si>
     <t>CLTV</t>
   </si>
   <si>
@@ -90,13 +87,16 @@
     <t>OwnershipGroupName</t>
   </si>
   <si>
-    <t>SalesGroupName</t>
-  </si>
-  <si>
     <t>Sales group 1</t>
   </si>
   <si>
     <t>Ownership group 1</t>
+  </si>
+  <si>
+    <t>TrueIND</t>
+  </si>
+  <si>
+    <t>RepFirm</t>
   </si>
 </sst>
 </file>
@@ -483,9 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC98319-C6D9-4A0F-8766-1F87946705E8}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -504,28 +502,28 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>20</v>
+      <c r="J1" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -533,22 +531,23 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -556,21 +555,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-      <c r="I3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>21</v>
+      <c r="I3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -578,29 +577,29 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>21</v>
+      <c r="I4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -608,25 +607,25 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>21</v>
+      <c r="I5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>